<commit_message>
Se agrega nuevo componente
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -2229,8 +2229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,10 +2344,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2355,7 +2355,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -2366,10 +2366,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2424,7 +2424,7 @@
         <v>42</v>
       </c>
       <c r="C17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3419,7 +3419,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregan cambios y se agregan nuevos daos (aun no terminados)
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -1047,7 +1047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
@@ -2229,8 +2229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,7 +2259,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2765,7 +2765,7 @@
         <v>65</v>
       </c>
       <c r="C48" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2809,7 +2809,7 @@
         <v>68</v>
       </c>
       <c r="C52" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2820,7 +2820,7 @@
         <v>69</v>
       </c>
       <c r="C53" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -2886,7 +2886,7 @@
         <v>73</v>
       </c>
       <c r="C59" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -3238,7 +3238,7 @@
         <v>102</v>
       </c>
       <c r="C91" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3293,7 +3293,7 @@
         <v>107</v>
       </c>
       <c r="C96" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="C109">
         <f>COUNTIFS(C2:C105,"&gt;"&amp; 0%,C2:C105,"&lt;" &amp; 100%)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -3419,7 +3419,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios realizados en daos y controllers para Préstamo
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -1047,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,7 +1729,7 @@
         <v>4</v>
       </c>
       <c r="C56" s="3">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="D56" s="3"/>
     </row>
@@ -2229,8 +2229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2688,7 +2688,7 @@
         <v>60</v>
       </c>
       <c r="C41" s="3">
-        <v>0</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="C109">
         <f>COUNTIFS(C2:C105,"&gt;"&amp; 0%,C2:C105,"&lt;" &amp; 100%)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -3419,7 +3419,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modifica archivo de avances y startup de controllers
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -1047,7 +1047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
@@ -1729,7 +1729,7 @@
         <v>4</v>
       </c>
       <c r="C56" s="3">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="D56" s="3"/>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="C96">
         <f>COUNTIFS(C2:C93,100%)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
@@ -2190,7 +2190,7 @@
       </c>
       <c r="C97">
         <f>COUNTIFS(C2:C93,"&gt;"&amp; 0%,C2:C93,"&lt;" &amp; 100%)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
@@ -2229,8 +2229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2842,7 +2842,7 @@
         <v>19</v>
       </c>
       <c r="C55" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -3007,7 +3007,7 @@
         <v>21</v>
       </c>
       <c r="C70" s="1">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="C109">
         <f>COUNTIFS(C2:C105,"&gt;"&amp; 0%,C2:C105,"&lt;" &amp; 100%)</f>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se realizan cambios en controlador de entidad
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -1047,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1074,7 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1086,7 +1086,7 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1098,7 +1098,7 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1110,7 +1110,7 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1122,7 +1122,7 @@
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1134,7 +1134,7 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -1146,7 +1146,7 @@
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1158,7 +1158,7 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1170,7 +1170,7 @@
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -1182,7 +1182,7 @@
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -1194,7 +1194,7 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -1206,7 +1206,7 @@
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -1218,7 +1218,7 @@
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -1230,7 +1230,7 @@
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -1242,7 +1242,7 @@
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -1254,7 +1254,7 @@
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -1266,7 +1266,7 @@
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -1278,7 +1278,7 @@
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -1290,7 +1290,7 @@
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -1302,7 +1302,7 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -1314,7 +1314,7 @@
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -1326,7 +1326,7 @@
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -1338,7 +1338,7 @@
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -1350,19 +1350,19 @@
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" t="s">
@@ -1374,7 +1374,7 @@
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -1386,7 +1386,7 @@
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" t="s">
@@ -1398,7 +1398,7 @@
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" t="s">
@@ -1410,7 +1410,7 @@
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" t="s">
@@ -1422,7 +1422,7 @@
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" t="s">
@@ -1434,7 +1434,7 @@
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" t="s">
@@ -1446,7 +1446,7 @@
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
       <c r="B33" t="s">
@@ -1458,7 +1458,7 @@
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
       <c r="B34" t="s">
@@ -1470,7 +1470,7 @@
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
       <c r="B35" t="s">
@@ -1482,7 +1482,7 @@
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="4">
         <v>35</v>
       </c>
       <c r="B36" t="s">
@@ -1494,7 +1494,7 @@
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="4">
         <v>36</v>
       </c>
       <c r="B37" t="s">
@@ -1506,7 +1506,7 @@
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="4">
         <v>37</v>
       </c>
       <c r="B38" t="s">
@@ -1518,7 +1518,7 @@
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="4">
         <v>38</v>
       </c>
       <c r="B39" t="s">
@@ -1530,7 +1530,7 @@
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="4">
         <v>39</v>
       </c>
       <c r="B40" t="s">
@@ -1542,7 +1542,7 @@
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="4">
         <v>40</v>
       </c>
       <c r="B41" t="s">
@@ -1554,7 +1554,7 @@
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="4">
         <v>41</v>
       </c>
       <c r="B42" t="s">
@@ -1566,7 +1566,7 @@
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="4">
         <v>42</v>
       </c>
       <c r="B43" t="s">
@@ -1578,7 +1578,7 @@
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="4">
         <v>43</v>
       </c>
       <c r="B44" t="s">
@@ -1590,7 +1590,7 @@
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="4">
         <v>44</v>
       </c>
       <c r="B45" t="s">
@@ -1602,7 +1602,7 @@
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="4">
         <v>45</v>
       </c>
       <c r="B46" t="s">
@@ -1614,7 +1614,7 @@
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="4">
         <v>46</v>
       </c>
       <c r="B47" t="s">
@@ -1626,7 +1626,7 @@
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="4">
         <v>47</v>
       </c>
       <c r="B48" t="s">
@@ -1638,7 +1638,7 @@
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="4">
         <v>48</v>
       </c>
       <c r="B49" t="s">
@@ -1650,7 +1650,7 @@
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="4">
         <v>49</v>
       </c>
       <c r="B50" t="s">
@@ -1662,7 +1662,7 @@
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="4">
         <v>50</v>
       </c>
       <c r="B51" t="s">
@@ -1674,7 +1674,7 @@
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="4">
         <v>51</v>
       </c>
       <c r="B52" t="s">
@@ -1686,7 +1686,7 @@
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="4">
         <v>52</v>
       </c>
       <c r="B53" t="s">
@@ -1698,7 +1698,7 @@
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="4">
         <v>53</v>
       </c>
       <c r="B54" t="s">
@@ -1710,7 +1710,7 @@
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="4">
         <v>54</v>
       </c>
       <c r="B55" t="s">
@@ -1722,7 +1722,7 @@
       <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="4">
         <v>55</v>
       </c>
       <c r="B56" t="s">
@@ -1734,7 +1734,7 @@
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="4">
         <v>56</v>
       </c>
       <c r="B57" t="s">
@@ -1746,7 +1746,7 @@
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="4">
         <v>57</v>
       </c>
       <c r="B58" t="s">
@@ -1758,7 +1758,7 @@
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="4">
         <v>58</v>
       </c>
       <c r="B59" t="s">
@@ -1770,7 +1770,7 @@
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="4">
         <v>59</v>
       </c>
       <c r="B60" t="s">
@@ -1782,7 +1782,7 @@
       <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="4">
         <v>60</v>
       </c>
       <c r="B61" t="s">
@@ -1794,7 +1794,7 @@
       <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="4">
         <v>61</v>
       </c>
       <c r="B62" t="s">
@@ -1806,7 +1806,7 @@
       <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="4">
         <v>62</v>
       </c>
       <c r="B63" t="s">
@@ -1818,7 +1818,7 @@
       <c r="D63" s="3"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="A64" s="4">
         <v>63</v>
       </c>
       <c r="B64" t="s">
@@ -1830,7 +1830,7 @@
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="A65" s="4">
         <v>64</v>
       </c>
       <c r="B65" t="s">
@@ -1842,7 +1842,7 @@
       <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
+      <c r="A66" s="4">
         <v>65</v>
       </c>
       <c r="B66" t="s">
@@ -1854,7 +1854,7 @@
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="A67" s="4">
         <v>66</v>
       </c>
       <c r="B67" t="s">
@@ -1866,7 +1866,7 @@
       <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68">
+      <c r="A68" s="4">
         <v>67</v>
       </c>
       <c r="B68" t="s">
@@ -1878,7 +1878,7 @@
       <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69">
+      <c r="A69" s="4">
         <v>68</v>
       </c>
       <c r="B69" t="s">
@@ -1890,7 +1890,7 @@
       <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70">
+      <c r="A70" s="4">
         <v>69</v>
       </c>
       <c r="B70" t="s">
@@ -1902,7 +1902,7 @@
       <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71">
+      <c r="A71" s="4">
         <v>70</v>
       </c>
       <c r="B71" t="s">
@@ -1914,7 +1914,7 @@
       <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72">
+      <c r="A72" s="4">
         <v>71</v>
       </c>
       <c r="B72" t="s">
@@ -1926,7 +1926,7 @@
       <c r="D72" s="3"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73">
+      <c r="A73" s="4">
         <v>72</v>
       </c>
       <c r="B73" t="s">
@@ -1938,7 +1938,7 @@
       <c r="D73" s="3"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74">
+      <c r="A74" s="4">
         <v>73</v>
       </c>
       <c r="B74" t="s">
@@ -1950,7 +1950,7 @@
       <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75">
+      <c r="A75" s="4">
         <v>74</v>
       </c>
       <c r="B75" t="s">
@@ -1962,7 +1962,7 @@
       <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76">
+      <c r="A76" s="4">
         <v>75</v>
       </c>
       <c r="B76" t="s">
@@ -1974,7 +1974,7 @@
       <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77">
+      <c r="A77" s="4">
         <v>76</v>
       </c>
       <c r="B77" t="s">
@@ -1986,7 +1986,7 @@
       <c r="D77" s="3"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78">
+      <c r="A78" s="4">
         <v>77</v>
       </c>
       <c r="B78" t="s">
@@ -1998,7 +1998,7 @@
       <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79">
+      <c r="A79" s="4">
         <v>78</v>
       </c>
       <c r="B79" t="s">
@@ -2010,7 +2010,7 @@
       <c r="D79" s="3"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80">
+      <c r="A80" s="4">
         <v>79</v>
       </c>
       <c r="B80" t="s">
@@ -2022,7 +2022,7 @@
       <c r="D80" s="3"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81">
+      <c r="A81" s="4">
         <v>80</v>
       </c>
       <c r="B81" t="s">
@@ -2034,7 +2034,7 @@
       <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82">
+      <c r="A82" s="4">
         <v>81</v>
       </c>
       <c r="B82" t="s">
@@ -2046,7 +2046,7 @@
       <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83">
+      <c r="A83" s="4">
         <v>82</v>
       </c>
       <c r="B83" t="s">
@@ -2058,7 +2058,7 @@
       <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84">
+      <c r="A84" s="4">
         <v>83</v>
       </c>
       <c r="B84" t="s">
@@ -2070,7 +2070,7 @@
       <c r="D84" s="3"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85">
+      <c r="A85" s="4">
         <v>84</v>
       </c>
       <c r="B85" t="s">
@@ -2082,7 +2082,7 @@
       <c r="D85" s="3"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86">
+      <c r="A86" s="4">
         <v>85</v>
       </c>
       <c r="B86" t="s">
@@ -2094,7 +2094,7 @@
       <c r="D86" s="3"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87">
+      <c r="A87" s="4">
         <v>86</v>
       </c>
       <c r="B87" t="s">
@@ -2106,7 +2106,7 @@
       <c r="D87" s="3"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88">
+      <c r="A88" s="4">
         <v>87</v>
       </c>
       <c r="B88" t="s">
@@ -2118,7 +2118,7 @@
       <c r="D88" s="3"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89">
+      <c r="A89" s="4">
         <v>88</v>
       </c>
       <c r="B89" t="s">
@@ -2130,7 +2130,7 @@
       <c r="D89" s="3"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90">
+      <c r="A90" s="4">
         <v>89</v>
       </c>
       <c r="B90" t="s">
@@ -2142,7 +2142,7 @@
       <c r="D90" s="3"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91">
+      <c r="A91" s="4">
         <v>90</v>
       </c>
       <c r="B91" t="s">
@@ -2154,7 +2154,7 @@
       <c r="D91" s="3"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92">
+      <c r="A92" s="4">
         <v>91</v>
       </c>
       <c r="B92" t="s">
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93">
+      <c r="A93" s="4">
         <v>92</v>
       </c>
       <c r="B93" t="s">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="C96">
         <f>COUNTIFS(C2:C93,100%)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C98">
         <f>COUNTIFS(C2:C93,0%)</f>
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2229,8 +2229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se realizan cambios en controllers
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1117,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="C96">
         <f>COUNTIFS(C2:C93,100%)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C98">
         <f>COUNTIFS(C2:C93,0%)</f>
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega controller de Autorización Tipo
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,7 +1153,7 @@
         <v>124</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="C96">
         <f>COUNTIFS(C2:C93,100%)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C98">
         <f>COUNTIFS(C2:C93,0%)</f>
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega controlador de data sigade y se hacen cambios en controladores existentes
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -1047,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1261,7 @@
         <v>132</v>
       </c>
       <c r="C17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="3"/>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="C96">
         <f>COUNTIFS(C2:C93,100%)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C98">
         <f>COUNTIFS(C2:C93,0%)</f>
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega controller de EjecucionEstado
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -1047,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,7 +1345,7 @@
         <v>139</v>
       </c>
       <c r="C24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="3"/>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="C96">
         <f>COUNTIFS(C2:C93,100%)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C98">
         <f>COUNTIFS(C2:C93,0%)</f>
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega controller de Interés Tipo
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,7 +1501,7 @@
         <v>151</v>
       </c>
       <c r="C37" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="3"/>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="C96">
         <f>COUNTIFS(C2:C93,100%)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C98">
         <f>COUNTIFS(C2:C93,0%)</f>
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregan cambios a daos para plan de adquisiciones
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -1047,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,7 +1657,7 @@
         <v>163</v>
       </c>
       <c r="C50" s="3">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D50" s="3"/>
     </row>
@@ -2190,7 +2190,7 @@
       </c>
       <c r="C97">
         <f>COUNTIFS(C2:C93,"&gt;"&amp; 0%,C2:C93,"&lt;" &amp; 100%)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C98">
         <f>COUNTIFS(C2:C93,0%)</f>
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2229,8 +2229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,7 +2259,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="3">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2358,7 +2358,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2820,7 +2820,7 @@
         <v>69</v>
       </c>
       <c r="C53" s="3">
-        <v>0.05</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3293,7 +3293,7 @@
         <v>107</v>
       </c>
       <c r="C96" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3348,7 +3348,7 @@
         <v>112</v>
       </c>
       <c r="C101" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3419,7 +3419,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se realizan cambios de autenticación en controllers
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="298">
   <si>
     <t>Controllers</t>
   </si>
@@ -634,6 +634,291 @@
   </si>
   <si>
     <t>SUsuario</t>
+  </si>
+  <si>
+    <t>Dirección/Puerto</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:59999</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60001</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60003</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60005</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60006</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60008</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60009</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60002</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60004</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60007</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60010</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60011</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60012</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60013</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60014</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60015</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60016</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60017</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60018</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60019</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60020</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60021</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60022</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60023</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60024</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60025</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60026</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60027</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60028</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60029</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60030</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60031</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60032</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60033</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60034</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60035</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60036</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60037</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60038</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60039</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60040</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60041</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60042</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60043</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60044</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60045</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60046</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60047</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60048</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60049</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60050</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60051</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60052</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60053</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60054</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60055</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60056</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60057</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60058</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60059</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60060</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60061</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60062</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60063</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60064</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60065</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60066</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60067</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60068</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60069</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60070</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60071</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60072</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60073</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60074</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60075</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60076</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60077</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60078</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60079</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60080</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60081</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60082</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60083</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60084</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60085</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60086</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60087</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60088</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60089</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60090</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60091</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:60000</t>
+  </si>
+  <si>
+    <t>Sipro Web</t>
   </si>
 </sst>
 </file>
@@ -685,7 +970,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -693,12 +978,22 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -769,8 +1064,43 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF99FF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1045,23 +1375,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>117</v>
       </c>
@@ -1069,1146 +1400,1453 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="C3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="C4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="C5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="C7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="C8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C9" t="s">
+        <v>213</v>
+      </c>
+      <c r="D9" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="C10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>126</v>
       </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="C11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="C12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="C13" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>129</v>
       </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="C14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>130</v>
       </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="C15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="C16" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C17" t="s">
+        <v>219</v>
+      </c>
+      <c r="D17" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C18" t="s">
+        <v>220</v>
+      </c>
+      <c r="D18" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="C19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="C20" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="C21" t="s">
+        <v>223</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>136</v>
       </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="C22" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="C23" t="s">
+        <v>225</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>138</v>
       </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="C24" t="s">
+        <v>226</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>139</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C25" t="s">
+        <v>227</v>
+      </c>
+      <c r="D25" s="3">
         <v>1</v>
       </c>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C26" t="s">
+        <v>228</v>
+      </c>
+      <c r="D26" s="3">
         <v>1</v>
       </c>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="C27" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>141</v>
       </c>
-      <c r="C27" s="3">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="C28" t="s">
+        <v>230</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="3">
-        <v>0</v>
-      </c>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="C29" t="s">
+        <v>231</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>143</v>
       </c>
-      <c r="C29" s="3">
-        <v>0</v>
-      </c>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="C30" t="s">
+        <v>232</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>144</v>
       </c>
-      <c r="C30" s="3">
-        <v>0</v>
-      </c>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="C31" t="s">
+        <v>233</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>145</v>
       </c>
-      <c r="C31" s="3">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="C32" t="s">
+        <v>234</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>146</v>
       </c>
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="C33" t="s">
+        <v>235</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>147</v>
       </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="C34" t="s">
+        <v>236</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="3">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="C35" t="s">
+        <v>237</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>149</v>
       </c>
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="C36" t="s">
+        <v>238</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>150</v>
       </c>
-      <c r="C36" s="3">
-        <v>0</v>
-      </c>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="C37" t="s">
+        <v>239</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>151</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C38" t="s">
+        <v>240</v>
+      </c>
+      <c r="D38" s="3">
         <v>1</v>
       </c>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C39" t="s">
+        <v>204</v>
+      </c>
+      <c r="D39" s="3">
         <v>1</v>
       </c>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>152</v>
       </c>
-      <c r="C39" s="3">
-        <v>0</v>
-      </c>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="C40" t="s">
+        <v>241</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>153</v>
       </c>
-      <c r="C40" s="3">
-        <v>0</v>
-      </c>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="C41" t="s">
+        <v>242</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>154</v>
       </c>
-      <c r="C41" s="3">
-        <v>0</v>
-      </c>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="C42" t="s">
+        <v>243</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>155</v>
       </c>
-      <c r="C42" s="3">
-        <v>0</v>
-      </c>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="C43" t="s">
+        <v>244</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="3">
-        <v>0</v>
-      </c>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="C44" t="s">
+        <v>245</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>157</v>
       </c>
-      <c r="C44" s="3">
-        <v>0</v>
-      </c>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="C45" t="s">
+        <v>246</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>158</v>
       </c>
-      <c r="C45" s="3">
-        <v>0</v>
-      </c>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="C46" t="s">
+        <v>247</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>159</v>
       </c>
-      <c r="C46" s="3">
-        <v>0</v>
-      </c>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="C47" t="s">
+        <v>248</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>160</v>
       </c>
-      <c r="C47" s="3">
-        <v>0</v>
-      </c>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="C48" t="s">
+        <v>249</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>161</v>
       </c>
-      <c r="C48" s="3">
-        <v>0</v>
-      </c>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+      <c r="C49" t="s">
+        <v>250</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>162</v>
       </c>
-      <c r="C49" s="3">
-        <v>0</v>
-      </c>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="C50" t="s">
+        <v>251</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>163</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C51" t="s">
+        <v>252</v>
+      </c>
+      <c r="D51" s="3">
         <v>0.6</v>
       </c>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>164</v>
       </c>
-      <c r="C51" s="3">
-        <v>0</v>
-      </c>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="C52" t="s">
+        <v>253</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0</v>
+      </c>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
         <v>51</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>165</v>
       </c>
-      <c r="C52" s="3">
-        <v>0</v>
-      </c>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="C53" t="s">
+        <v>254</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0</v>
+      </c>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
         <v>52</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>166</v>
       </c>
-      <c r="C53" s="3">
-        <v>0</v>
-      </c>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="C54" t="s">
+        <v>255</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
         <v>53</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>167</v>
       </c>
-      <c r="C54" s="3">
-        <v>0</v>
-      </c>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+      <c r="C55" t="s">
+        <v>256</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0</v>
+      </c>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>168</v>
       </c>
-      <c r="C55" s="3">
-        <v>0</v>
-      </c>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="C56" t="s">
+        <v>257</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0</v>
+      </c>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
         <v>55</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>4</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C57" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" s="3">
         <v>1</v>
       </c>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>169</v>
       </c>
-      <c r="C57" s="3">
-        <v>0</v>
-      </c>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+      <c r="C58" t="s">
+        <v>259</v>
+      </c>
+      <c r="D58" s="3">
+        <v>0</v>
+      </c>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
         <v>57</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>170</v>
       </c>
-      <c r="C58" s="3">
-        <v>0</v>
-      </c>
-      <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+      <c r="C59" t="s">
+        <v>260</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
         <v>58</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C60" t="s">
+        <v>261</v>
+      </c>
+      <c r="D60" s="3">
         <v>1</v>
       </c>
-      <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>171</v>
       </c>
-      <c r="C60" s="3">
-        <v>0</v>
-      </c>
-      <c r="D60" s="3"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+      <c r="C61" t="s">
+        <v>262</v>
+      </c>
+      <c r="D61" s="3">
+        <v>0</v>
+      </c>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
         <v>60</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>172</v>
       </c>
-      <c r="C61" s="3">
-        <v>0</v>
-      </c>
-      <c r="D61" s="3"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+      <c r="C62" t="s">
+        <v>263</v>
+      </c>
+      <c r="D62" s="3">
+        <v>0</v>
+      </c>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>173</v>
       </c>
-      <c r="C62" s="3">
-        <v>0</v>
-      </c>
-      <c r="D62" s="3"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+      <c r="C63" t="s">
+        <v>264</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0</v>
+      </c>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
         <v>62</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>174</v>
       </c>
-      <c r="C63" s="3">
-        <v>0</v>
-      </c>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+      <c r="C64" t="s">
+        <v>265</v>
+      </c>
+      <c r="D64" s="3">
+        <v>0</v>
+      </c>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
         <v>63</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>175</v>
       </c>
-      <c r="C64" s="3">
-        <v>0</v>
-      </c>
-      <c r="D64" s="3"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+      <c r="C65" t="s">
+        <v>266</v>
+      </c>
+      <c r="D65" s="3">
+        <v>0</v>
+      </c>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>176</v>
       </c>
-      <c r="C65" s="3">
-        <v>0</v>
-      </c>
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="C66" t="s">
+        <v>267</v>
+      </c>
+      <c r="D66" s="3">
+        <v>0</v>
+      </c>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
         <v>65</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>177</v>
       </c>
-      <c r="C66" s="3">
-        <v>0</v>
-      </c>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+      <c r="C67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D67" s="3">
+        <v>0</v>
+      </c>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
         <v>66</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>178</v>
       </c>
-      <c r="C67" s="3">
-        <v>0</v>
-      </c>
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+      <c r="C68" t="s">
+        <v>269</v>
+      </c>
+      <c r="D68" s="3">
+        <v>0</v>
+      </c>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
         <v>67</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>179</v>
       </c>
-      <c r="C68" s="3">
-        <v>0</v>
-      </c>
-      <c r="D68" s="3"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+      <c r="C69" t="s">
+        <v>270</v>
+      </c>
+      <c r="D69" s="3">
+        <v>0</v>
+      </c>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
         <v>68</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>180</v>
       </c>
-      <c r="C69" s="3">
-        <v>0</v>
-      </c>
-      <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+      <c r="C70" t="s">
+        <v>271</v>
+      </c>
+      <c r="D70" s="3">
+        <v>0</v>
+      </c>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
         <v>69</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>181</v>
       </c>
-      <c r="C70" s="3">
-        <v>0</v>
-      </c>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
+      <c r="C71" t="s">
+        <v>272</v>
+      </c>
+      <c r="D71" s="3">
+        <v>0</v>
+      </c>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
         <v>70</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>182</v>
       </c>
-      <c r="C71" s="3">
-        <v>0</v>
-      </c>
-      <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
+      <c r="C72" t="s">
+        <v>273</v>
+      </c>
+      <c r="D72" s="3">
+        <v>0</v>
+      </c>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
         <v>71</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>183</v>
       </c>
-      <c r="C72" s="3">
-        <v>0</v>
-      </c>
-      <c r="D72" s="3"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+      <c r="C73" t="s">
+        <v>274</v>
+      </c>
+      <c r="D73" s="3">
+        <v>0</v>
+      </c>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
         <v>72</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>184</v>
       </c>
-      <c r="C73" s="3">
-        <v>0</v>
-      </c>
-      <c r="D73" s="3"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+      <c r="C74" t="s">
+        <v>275</v>
+      </c>
+      <c r="D74" s="3">
+        <v>0</v>
+      </c>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
         <v>73</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>185</v>
       </c>
-      <c r="C74" s="3">
-        <v>0</v>
-      </c>
-      <c r="D74" s="3"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+      <c r="C75" t="s">
+        <v>276</v>
+      </c>
+      <c r="D75" s="3">
+        <v>0</v>
+      </c>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
         <v>74</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>186</v>
       </c>
-      <c r="C75" s="3">
-        <v>0</v>
-      </c>
-      <c r="D75" s="3"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
+      <c r="C76" t="s">
+        <v>277</v>
+      </c>
+      <c r="D76" s="3">
+        <v>0</v>
+      </c>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
         <v>75</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>187</v>
       </c>
-      <c r="C76" s="3">
-        <v>0</v>
-      </c>
-      <c r="D76" s="3"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
+      <c r="C77" t="s">
+        <v>278</v>
+      </c>
+      <c r="D77" s="3">
+        <v>0</v>
+      </c>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
         <v>76</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>188</v>
       </c>
-      <c r="C77" s="3">
-        <v>0</v>
-      </c>
-      <c r="D77" s="3"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
+      <c r="C78" t="s">
+        <v>279</v>
+      </c>
+      <c r="D78" s="3">
+        <v>0</v>
+      </c>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
         <v>77</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>189</v>
       </c>
-      <c r="C78" s="3">
-        <v>0</v>
-      </c>
-      <c r="D78" s="3"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="4">
+      <c r="C79" t="s">
+        <v>280</v>
+      </c>
+      <c r="D79" s="3">
+        <v>0</v>
+      </c>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
         <v>78</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>190</v>
       </c>
-      <c r="C79" s="3">
-        <v>0</v>
-      </c>
-      <c r="D79" s="3"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="4">
+      <c r="C80" t="s">
+        <v>281</v>
+      </c>
+      <c r="D80" s="3">
+        <v>0</v>
+      </c>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
         <v>79</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>191</v>
       </c>
-      <c r="C80" s="3">
-        <v>0</v>
-      </c>
-      <c r="D80" s="3"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="4">
+      <c r="C81" t="s">
+        <v>282</v>
+      </c>
+      <c r="D81" s="3">
+        <v>0</v>
+      </c>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
         <v>80</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>192</v>
       </c>
-      <c r="C81" s="3">
-        <v>0</v>
-      </c>
-      <c r="D81" s="3"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="4">
+      <c r="C82" t="s">
+        <v>283</v>
+      </c>
+      <c r="D82" s="3">
+        <v>0</v>
+      </c>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
         <v>81</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>193</v>
       </c>
-      <c r="C82" s="3">
-        <v>0</v>
-      </c>
-      <c r="D82" s="3"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
+      <c r="C83" t="s">
+        <v>284</v>
+      </c>
+      <c r="D83" s="3">
+        <v>0</v>
+      </c>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
         <v>82</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>194</v>
       </c>
-      <c r="C83" s="3">
-        <v>0</v>
-      </c>
-      <c r="D83" s="3"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="4">
+      <c r="C84" t="s">
+        <v>285</v>
+      </c>
+      <c r="D84" s="3">
+        <v>0</v>
+      </c>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
         <v>83</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>195</v>
       </c>
-      <c r="C84" s="3">
-        <v>0</v>
-      </c>
-      <c r="D84" s="3"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
+      <c r="C85" t="s">
+        <v>286</v>
+      </c>
+      <c r="D85" s="3">
+        <v>0</v>
+      </c>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
         <v>84</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>196</v>
       </c>
-      <c r="C85" s="3">
-        <v>0</v>
-      </c>
-      <c r="D85" s="3"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="4">
+      <c r="C86" t="s">
+        <v>287</v>
+      </c>
+      <c r="D86" s="3">
+        <v>0</v>
+      </c>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
         <v>85</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>197</v>
       </c>
-      <c r="C86" s="3">
-        <v>0</v>
-      </c>
-      <c r="D86" s="3"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
+      <c r="C87" t="s">
+        <v>288</v>
+      </c>
+      <c r="D87" s="3">
+        <v>0</v>
+      </c>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
         <v>86</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>198</v>
       </c>
-      <c r="C87" s="3">
-        <v>0</v>
-      </c>
-      <c r="D87" s="3"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
+      <c r="C88" t="s">
+        <v>289</v>
+      </c>
+      <c r="D88" s="3">
+        <v>0</v>
+      </c>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
         <v>87</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>199</v>
       </c>
-      <c r="C88" s="3">
-        <v>0</v>
-      </c>
-      <c r="D88" s="3"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
+      <c r="C89" t="s">
+        <v>290</v>
+      </c>
+      <c r="D89" s="3">
+        <v>0</v>
+      </c>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
         <v>88</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>200</v>
       </c>
-      <c r="C89" s="3">
-        <v>0</v>
-      </c>
-      <c r="D89" s="3"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
+      <c r="C90" t="s">
+        <v>291</v>
+      </c>
+      <c r="D90" s="3">
+        <v>0</v>
+      </c>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
         <v>89</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>6</v>
       </c>
-      <c r="C90" s="3">
+      <c r="C91" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D91" s="3">
         <v>1</v>
       </c>
-      <c r="D90" s="3"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
         <v>90</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>7</v>
       </c>
-      <c r="C91" s="3">
+      <c r="C92" t="s">
+        <v>293</v>
+      </c>
+      <c r="D92" s="3">
         <v>1</v>
       </c>
-      <c r="D91" s="3"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
         <v>91</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>201</v>
       </c>
-      <c r="C92" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
+      <c r="C93" t="s">
+        <v>294</v>
+      </c>
+      <c r="D93" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
         <v>92</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>202</v>
       </c>
-      <c r="C93" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
+      <c r="C94" t="s">
+        <v>295</v>
+      </c>
+      <c r="D94" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C96">
-        <f>COUNTIFS(C2:C93,100%)</f>
+      <c r="C97" s="4"/>
+      <c r="D97">
+        <f>COUNTIFS(D3:D94,100%)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="4" t="s">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C97">
-        <f>COUNTIFS(C2:C93,"&gt;"&amp; 0%,C2:C93,"&lt;" &amp; 100%)</f>
+      <c r="C98" s="4"/>
+      <c r="D98">
+        <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C98">
-        <f>COUNTIFS(C2:C93,0%)</f>
+      <c r="C99" s="4"/>
+      <c r="D99">
+        <f>COUNTIFS(D3:D94,0%)</f>
         <v>79</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C93">
+  <conditionalFormatting sqref="D3:D94">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="between">
+      <formula>0.01</formula>
+      <formula>0.99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C91">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -2221,7 +2859,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Cambios en controller de Plan de Adquisiciones
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
     <sheet name="Daos" sheetId="2" r:id="rId2"/>
+    <sheet name="Vistas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1377,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2151,7 +2152,7 @@
         <v>252</v>
       </c>
       <c r="D51" s="3">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E51" s="3"/>
     </row>
@@ -2805,7 +2806,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -2815,7 +2816,7 @@
       <c r="C98" s="4"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -2867,8 +2868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3447,7 +3448,7 @@
         <v>68</v>
       </c>
       <c r="C52" s="3">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -3524,7 +3525,7 @@
         <v>73</v>
       </c>
       <c r="C59" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -4039,7 +4040,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4048,7 +4049,7 @@
       </c>
       <c r="C109">
         <f>COUNTIFS(C2:C105,"&gt;"&amp; 0%,C2:C105,"&lt;" &amp; 100%)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -4076,4 +4077,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Creación y avances en Plan de Adquisiciones Pagos
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
     <sheet name="Daos" sheetId="2" r:id="rId2"/>
     <sheet name="Vistas" sheetId="3" r:id="rId3"/>
+    <sheet name="Avance" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="314">
   <si>
     <t>Controllers</t>
   </si>
@@ -920,13 +921,61 @@
   </si>
   <si>
     <t>Sipro Web</t>
+  </si>
+  <si>
+    <t>SIPRO - Migración a estandar DTI</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Completados</t>
+  </si>
+  <si>
+    <t>% de avance</t>
+  </si>
+  <si>
+    <t>Dias de trabajo estimado (1 persona)</t>
+  </si>
+  <si>
+    <t>Dias de avance</t>
+  </si>
+  <si>
+    <t>Instalación de ambiente de trabajo en computadoras personales</t>
+  </si>
+  <si>
+    <t>Definición de arquitectura de software a implementar</t>
+  </si>
+  <si>
+    <t>Implementación de estructura básica de arquitectura de software</t>
+  </si>
+  <si>
+    <t>Programación de POCOs</t>
+  </si>
+  <si>
+    <t>Programación de DAOs</t>
+  </si>
+  <si>
+    <t>Programación de Controllers</t>
+  </si>
+  <si>
+    <t>Programación de POCOs Analytic</t>
+  </si>
+  <si>
+    <t>Programación de Vista</t>
+  </si>
+  <si>
+    <t>Totales</t>
+  </si>
+  <si>
+    <t>Avance Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -949,6 +998,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -958,7 +1022,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -966,12 +1030,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -988,6 +1067,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1378,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2182,7 +2274,7 @@
         <v>254</v>
       </c>
       <c r="D53" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" s="3"/>
     </row>
@@ -2806,7 +2898,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -2826,7 +2918,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2869,7 +2961,7 @@
   <dimension ref="A1:C110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3459,7 +3551,7 @@
         <v>69</v>
       </c>
       <c r="C53" s="3">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -4040,7 +4132,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4049,7 +4141,7 @@
       </c>
       <c r="C109">
         <f>COUNTIFS(C2:C105,"&gt;"&amp; 0%,C2:C105,"&lt;" &amp; 100%)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -4083,10 +4175,262 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11">
+        <f>D4/C4</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="9">
+        <v>3</v>
+      </c>
+      <c r="G4" s="12">
+        <f t="shared" ref="G4:G11" si="0">F4*E4</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" ref="E5:E11" si="1">D5/C5</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="9">
+        <v>5</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="9">
+        <v>5</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="C7" s="9">
+        <v>101</v>
+      </c>
+      <c r="D7" s="9">
+        <v>101</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="9">
+        <v>8</v>
+      </c>
+      <c r="G7" s="12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C8" s="9">
+        <f>Daos!A105</f>
+        <v>104</v>
+      </c>
+      <c r="D8" s="9">
+        <f>Daos!C108</f>
+        <v>21</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="1"/>
+        <v>0.20192307692307693</v>
+      </c>
+      <c r="F8" s="9">
+        <v>20</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="0"/>
+        <v>4.0384615384615383</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C9" s="9">
+        <f>Controllers!A94</f>
+        <v>92</v>
+      </c>
+      <c r="D9" s="9">
+        <f>Controllers!D97</f>
+        <v>14</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="1"/>
+        <v>0.15217391304347827</v>
+      </c>
+      <c r="F9" s="9">
+        <v>40</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" si="0"/>
+        <v>6.0869565217391308</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C10" s="9">
+        <v>12</v>
+      </c>
+      <c r="D10" s="9">
+        <v>12</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>8</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="C11" s="9">
+        <v>83</v>
+      </c>
+      <c r="D11" s="9">
+        <v>4</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" si="1"/>
+        <v>4.8192771084337352E-2</v>
+      </c>
+      <c r="F11" s="9">
+        <v>120</v>
+      </c>
+      <c r="G11" s="12">
+        <f t="shared" si="0"/>
+        <v>5.7831325301204819</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9">
+        <f>SUM(F4:F11)</f>
+        <v>209</v>
+      </c>
+      <c r="G12" s="12">
+        <f>SUM(G4:G11)</f>
+        <v>44.908550590321155</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="B15" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="C15" s="15">
+        <f>G12/F12</f>
+        <v>0.21487344780057968</v>
+      </c>
+      <c r="D15" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C15:D15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
migración de cambios para html de prestamo
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="497">
   <si>
     <t>Controllers</t>
   </si>
@@ -979,6 +979,546 @@
   </si>
   <si>
     <t>Vistas</t>
+  </si>
+  <si>
+    <t>ActividadValidator</t>
+  </si>
+  <si>
+    <t>ActividadPropiedadValidator</t>
+  </si>
+  <si>
+    <t>ActividadPropiedadValorValidator</t>
+  </si>
+  <si>
+    <t>ActividadTipoValidator</t>
+  </si>
+  <si>
+    <t>ActividadUsuarioValidator</t>
+  </si>
+  <si>
+    <t>AcumulacionCostoValidator</t>
+  </si>
+  <si>
+    <t>AsignacionRaciValidator</t>
+  </si>
+  <si>
+    <t>AtipoPropiedadValidator</t>
+  </si>
+  <si>
+    <t>AutorizacionTipoValidator</t>
+  </si>
+  <si>
+    <t>CategoriaAdquisicionValidator</t>
+  </si>
+  <si>
+    <t>ColaboradorValidator</t>
+  </si>
+  <si>
+    <t>ComponentePropiedadValidator</t>
+  </si>
+  <si>
+    <t>ComponentePropiedadValorValidator</t>
+  </si>
+  <si>
+    <t>ComponenteSigadeValidator</t>
+  </si>
+  <si>
+    <t>ComponenteTipoValidator</t>
+  </si>
+  <si>
+    <t>ComponenteUsuarioValidator</t>
+  </si>
+  <si>
+    <t>ComponenteValidator</t>
+  </si>
+  <si>
+    <t>CooperanteValidator</t>
+  </si>
+  <si>
+    <t>CtipoPropiedadValidator</t>
+  </si>
+  <si>
+    <t>DatoTipoValidator</t>
+  </si>
+  <si>
+    <t>DesembolsoTipoValidator</t>
+  </si>
+  <si>
+    <t>DesembolsoValidator</t>
+  </si>
+  <si>
+    <t>DocumentoValidator</t>
+  </si>
+  <si>
+    <t>EjecucionEstadoValidator</t>
+  </si>
+  <si>
+    <t>EntidadValidator</t>
+  </si>
+  <si>
+    <t>EstadoTablaValidator</t>
+  </si>
+  <si>
+    <t>EstadoValidator</t>
+  </si>
+  <si>
+    <t>EtiquetaValidator</t>
+  </si>
+  <si>
+    <t>FormularioItemOpcionValidator</t>
+  </si>
+  <si>
+    <t>FormularioItemTipoValidator</t>
+  </si>
+  <si>
+    <t>FormularioItemValidator</t>
+  </si>
+  <si>
+    <t>FormularioItemValorValidator</t>
+  </si>
+  <si>
+    <t>FormularioTipoValidator</t>
+  </si>
+  <si>
+    <t>FormularioValidator</t>
+  </si>
+  <si>
+    <t>HitoResultadoValidator</t>
+  </si>
+  <si>
+    <t>HitoTipoValidator</t>
+  </si>
+  <si>
+    <t>HitoValidator</t>
+  </si>
+  <si>
+    <t>InteresTipoValidator</t>
+  </si>
+  <si>
+    <t>LineaBaseValidator</t>
+  </si>
+  <si>
+    <t>MatrizRaciValidator</t>
+  </si>
+  <si>
+    <t>MetaAvanceValidator</t>
+  </si>
+  <si>
+    <t>MetaTipoValidator</t>
+  </si>
+  <si>
+    <t>MetaUnidadMedidaValidator</t>
+  </si>
+  <si>
+    <t>MetaValidator</t>
+  </si>
+  <si>
+    <t>MetaValorValidator</t>
+  </si>
+  <si>
+    <t>ObjetoFormularioValidator</t>
+  </si>
+  <si>
+    <t>ObjetoRiesgoValidator</t>
+  </si>
+  <si>
+    <t>PagoPlanificadoValidator</t>
+  </si>
+  <si>
+    <t>PepDetalleValidator</t>
+  </si>
+  <si>
+    <t>PermisoValidator</t>
+  </si>
+  <si>
+    <t>PlanAdquisicionPagoValidator</t>
+  </si>
+  <si>
+    <t>PlanAdquisicionValidator</t>
+  </si>
+  <si>
+    <t>PrestamoTipoPrestamoValidator</t>
+  </si>
+  <si>
+    <t>PrestamoTipoValidator</t>
+  </si>
+  <si>
+    <t>PrestamoUsuarioValidator</t>
+  </si>
+  <si>
+    <t>ProdtipoPropiedadValidator</t>
+  </si>
+  <si>
+    <t>ProductoPropiedadValidator</t>
+  </si>
+  <si>
+    <t>ProductoPropiedadValorValidator</t>
+  </si>
+  <si>
+    <t>ProductoTipoValidator</t>
+  </si>
+  <si>
+    <t>ProductoUsuarioValidator</t>
+  </si>
+  <si>
+    <t>ProductoValidator</t>
+  </si>
+  <si>
+    <t>ProyectoImpactoValidator</t>
+  </si>
+  <si>
+    <t>ProyectoMiembroValidator</t>
+  </si>
+  <si>
+    <t>ProyectoPropiedadValidator</t>
+  </si>
+  <si>
+    <t>ProyectoPropiedadValorValidator</t>
+  </si>
+  <si>
+    <t>ProyectoRolColaboradorValidator</t>
+  </si>
+  <si>
+    <t>ProyectoTipoValidator</t>
+  </si>
+  <si>
+    <t>ProyectoUsuarioValidator</t>
+  </si>
+  <si>
+    <t>ProyectoValidator</t>
+  </si>
+  <si>
+    <t>PtipoPropiedadValidator</t>
+  </si>
+  <si>
+    <t>RiesgoPropiedadValidator</t>
+  </si>
+  <si>
+    <t>RiesgoPropiedadValorValidator</t>
+  </si>
+  <si>
+    <t>RiesgoTipoValidator</t>
+  </si>
+  <si>
+    <t>RiesgoValidator</t>
+  </si>
+  <si>
+    <t>RolPermisoValidator</t>
+  </si>
+  <si>
+    <t>RolUnidadEjecutoraValidator</t>
+  </si>
+  <si>
+    <t>RolUsuarioProyectoValidator</t>
+  </si>
+  <si>
+    <t>RolValidator</t>
+  </si>
+  <si>
+    <t>RtipoPropiedadValidator</t>
+  </si>
+  <si>
+    <t>SctipoPropiedadValidator</t>
+  </si>
+  <si>
+    <t>SubcomponentePropiedadValidator</t>
+  </si>
+  <si>
+    <t>SubcomponentePropiedadValorValidator</t>
+  </si>
+  <si>
+    <t>SubcomponenteTipoValidator</t>
+  </si>
+  <si>
+    <t>SubcomponenteUsuarioValidator</t>
+  </si>
+  <si>
+    <t>SubcomponenteValidator</t>
+  </si>
+  <si>
+    <t>SubprodtipoPropiedadValidator</t>
+  </si>
+  <si>
+    <t>SubproductoPropiedadValidator</t>
+  </si>
+  <si>
+    <t>SubproductoPropiedadValorValidator</t>
+  </si>
+  <si>
+    <t>SubproductoTipoValidator</t>
+  </si>
+  <si>
+    <t>SubproductoUsuarioValidator</t>
+  </si>
+  <si>
+    <t>SubproductoValidator</t>
+  </si>
+  <si>
+    <t>TipoAdquisicionValidator</t>
+  </si>
+  <si>
+    <t>TipoMonedaValidator</t>
+  </si>
+  <si>
+    <t>UnidadEjecutoraValidator</t>
+  </si>
+  <si>
+    <t>UnidadMedidaValidator</t>
+  </si>
+  <si>
+    <t>UsuarioLogValidator</t>
+  </si>
+  <si>
+    <t>UsuarioPermisoValidator</t>
+  </si>
+  <si>
+    <t>UsuarioValidator</t>
+  </si>
+  <si>
+    <t>PrestamoValidator</t>
+  </si>
+  <si>
+    <t>MetaPlanificadoValidator</t>
+  </si>
+  <si>
+    <t>actividad</t>
+  </si>
+  <si>
+    <t>actividadpropiedad</t>
+  </si>
+  <si>
+    <t>actividadtipo</t>
+  </si>
+  <si>
+    <t>adquisicion</t>
+  </si>
+  <si>
+    <t>categoriaadquisicion</t>
+  </si>
+  <si>
+    <t>colaborador</t>
+  </si>
+  <si>
+    <t>componente</t>
+  </si>
+  <si>
+    <t>componentepropiedad</t>
+  </si>
+  <si>
+    <t>componentetipo</t>
+  </si>
+  <si>
+    <t>cooperante</t>
+  </si>
+  <si>
+    <t>desembolso</t>
+  </si>
+  <si>
+    <t>dialogoconfirmacion</t>
+  </si>
+  <si>
+    <t>documentosadjuntos</t>
+  </si>
+  <si>
+    <t>entidades</t>
+  </si>
+  <si>
+    <t>formulario</t>
+  </si>
+  <si>
+    <t>formularioitemtipo</t>
+  </si>
+  <si>
+    <t>formulariotipo</t>
+  </si>
+  <si>
+    <t>gantt</t>
+  </si>
+  <si>
+    <t>historia</t>
+  </si>
+  <si>
+    <t>hito</t>
+  </si>
+  <si>
+    <t>hitotipo</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>main_treeview</t>
+  </si>
+  <si>
+    <t>mapas</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>metatipo</t>
+  </si>
+  <si>
+    <t>metavalor</t>
+  </si>
+  <si>
+    <t>miembrosunidadejecutora</t>
+  </si>
+  <si>
+    <t>pago_planificado</t>
+  </si>
+  <si>
+    <t>pep</t>
+  </si>
+  <si>
+    <t>peppropiedad</t>
+  </si>
+  <si>
+    <t>permiso</t>
+  </si>
+  <si>
+    <t>prestamo</t>
+  </si>
+  <si>
+    <t>producto</t>
+  </si>
+  <si>
+    <t>productopropiedad</t>
+  </si>
+  <si>
+    <t>productotipo</t>
+  </si>
+  <si>
+    <t>programapropiedad</t>
+  </si>
+  <si>
+    <t>programatipo</t>
+  </si>
+  <si>
+    <t>recurso</t>
+  </si>
+  <si>
+    <t>recursopropiedad</t>
+  </si>
+  <si>
+    <t>recursotipo</t>
+  </si>
+  <si>
+    <t>recursounidadmedida</t>
+  </si>
+  <si>
+    <t>responsablerol</t>
+  </si>
+  <si>
+    <t>responsabletipo</t>
+  </si>
+  <si>
+    <t>riesgo</t>
+  </si>
+  <si>
+    <t>riesgopropiedad</t>
+  </si>
+  <si>
+    <t>riesgotipo</t>
+  </si>
+  <si>
+    <t>rolunidadejecutora</t>
+  </si>
+  <si>
+    <t>subcomponente</t>
+  </si>
+  <si>
+    <t>subcomponentepropiedad</t>
+  </si>
+  <si>
+    <t>subcomponentetipo</t>
+  </si>
+  <si>
+    <t>subproducto</t>
+  </si>
+  <si>
+    <t>subproductopropiedad</t>
+  </si>
+  <si>
+    <t>subproductotipo</t>
+  </si>
+  <si>
+    <t>tipoadquisicion</t>
+  </si>
+  <si>
+    <t>unidadejecutora</t>
+  </si>
+  <si>
+    <t>unidadmedida</t>
+  </si>
+  <si>
+    <t>usuarios</t>
+  </si>
+  <si>
+    <t>utilidades</t>
+  </si>
+  <si>
+    <t>reportes/administraciontransaccional</t>
+  </si>
+  <si>
+    <t>reportes/agenda</t>
+  </si>
+  <si>
+    <t>reportes/avanceactividades</t>
+  </si>
+  <si>
+    <t>reportes/cargatrabajo</t>
+  </si>
+  <si>
+    <t>reportes/desembolsos</t>
+  </si>
+  <si>
+    <t>reportes/flujocaja</t>
+  </si>
+  <si>
+    <t>reportes/gestionadquisiciones</t>
+  </si>
+  <si>
+    <t>reportes/informacionPresupuestaria</t>
+  </si>
+  <si>
+    <t>reportes/informeGeneralPEP</t>
+  </si>
+  <si>
+    <t>reportes/jasper</t>
+  </si>
+  <si>
+    <t>reportes/matrizraci</t>
+  </si>
+  <si>
+    <t>reportes/matrizriesgo</t>
+  </si>
+  <si>
+    <t>reportes/planadquisiciones</t>
+  </si>
+  <si>
+    <t>reportes/planejecucion</t>
+  </si>
+  <si>
+    <t>reportes/planestructuraproyecto</t>
+  </si>
+  <si>
+    <t>reportes/porcentajeactividades</t>
+  </si>
+  <si>
+    <t>reportes/prestamoindicadores</t>
+  </si>
+  <si>
+    <t>reportes/prestamometas</t>
+  </si>
+  <si>
+    <t>reportes/reportefinancieroadquisiciones</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1636,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1510,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97:D99"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,7 +3094,7 @@
         <v>268</v>
       </c>
       <c r="D67" s="3">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E67" s="3"/>
     </row>
@@ -2938,7 +3508,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -2948,7 +3518,7 @@
       <c r="C98" s="4"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -2963,31 +3533,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D94">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="between">
       <formula>0.01</formula>
       <formula>0.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>0.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3000,8 +3570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108:C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3778,7 +4348,7 @@
         <v>21</v>
       </c>
       <c r="C70" s="1">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -4195,6 +4765,957 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C105">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
+      <formula>0.01</formula>
+      <formula>0.99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C86"/>
+  <sheetViews>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>419</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>420</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>422</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>424</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>425</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>426</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>427</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>428</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>429</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>430</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>431</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>432</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>433</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>434</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>435</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>436</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>437</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>438</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>439</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>440</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>441</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>442</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>443</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>444</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>445</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>446</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>447</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>448</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>449</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>450</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>451</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>452</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>453</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>454</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>455</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>456</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>457</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>458</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>459</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>460</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>478</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>479</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>480</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>481</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>482</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>483</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>484</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>485</v>
+      </c>
+      <c r="C53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>486</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>487</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>488</v>
+      </c>
+      <c r="C56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>489</v>
+      </c>
+      <c r="C57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>490</v>
+      </c>
+      <c r="C58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>491</v>
+      </c>
+      <c r="C59" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>492</v>
+      </c>
+      <c r="C60" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>493</v>
+      </c>
+      <c r="C61" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>494</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>495</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>496</v>
+      </c>
+      <c r="C64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>461</v>
+      </c>
+      <c r="C65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>462</v>
+      </c>
+      <c r="C66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>463</v>
+      </c>
+      <c r="C67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>464</v>
+      </c>
+      <c r="C68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>465</v>
+      </c>
+      <c r="C69" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>466</v>
+      </c>
+      <c r="C70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>467</v>
+      </c>
+      <c r="C71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>468</v>
+      </c>
+      <c r="C72" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>469</v>
+      </c>
+      <c r="C73" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>470</v>
+      </c>
+      <c r="C74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>471</v>
+      </c>
+      <c r="C75" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>472</v>
+      </c>
+      <c r="C76" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>473</v>
+      </c>
+      <c r="C77" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>474</v>
+      </c>
+      <c r="C78" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>475</v>
+      </c>
+      <c r="C79" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>476</v>
+      </c>
+      <c r="C80" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>477</v>
+      </c>
+      <c r="C81" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C84">
+        <f>COUNTIFS(C2:C81,100%)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C85">
+        <f>COUNTIFS(C2:C81,"&gt;"&amp; 0%,C2:C81,"&lt;" &amp; 100%)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C86">
+        <f>COUNTIFS(C2:C81,0%)</f>
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C81">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4207,46 +5728,16 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4271,7 +5762,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>318</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -4282,7 +5773,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>319</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -4293,7 +5784,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>320</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -4304,7 +5795,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>321</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -4315,7 +5806,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>317</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -4326,7 +5817,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>322</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -4337,7 +5828,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>323</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -4348,7 +5839,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>324</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -4359,7 +5850,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>325</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -4370,7 +5861,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>326</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -4381,7 +5872,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>327</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -4392,7 +5883,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>328</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -4403,7 +5894,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>329</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -4414,7 +5905,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>330</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -4425,7 +5916,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>331</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -4436,7 +5927,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>132</v>
+        <v>332</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -4447,7 +5938,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>333</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
@@ -4458,7 +5949,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>334</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -4469,7 +5960,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>135</v>
+        <v>335</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
@@ -4480,7 +5971,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>336</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
@@ -4491,7 +5982,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>337</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
@@ -4502,7 +5993,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>138</v>
+        <v>338</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -4513,7 +6004,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>339</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -4524,7 +6015,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>340</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
@@ -4535,7 +6026,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>341</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -4546,7 +6037,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>342</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -4557,7 +6048,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>142</v>
+        <v>343</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
@@ -4568,7 +6059,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>143</v>
+        <v>344</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
@@ -4579,7 +6070,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>345</v>
       </c>
       <c r="C30" s="3">
         <v>1</v>
@@ -4590,7 +6081,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>145</v>
+        <v>346</v>
       </c>
       <c r="C31" s="3">
         <v>1</v>
@@ -4601,7 +6092,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>347</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
@@ -4612,7 +6103,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>147</v>
+        <v>348</v>
       </c>
       <c r="C33" s="3">
         <v>1</v>
@@ -4623,7 +6114,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>148</v>
+        <v>349</v>
       </c>
       <c r="C34" s="3">
         <v>1</v>
@@ -4634,7 +6125,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>350</v>
       </c>
       <c r="C35" s="3">
         <v>1</v>
@@ -4645,7 +6136,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>351</v>
       </c>
       <c r="C36" s="3">
         <v>1</v>
@@ -4656,7 +6147,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>352</v>
       </c>
       <c r="C37" s="3">
         <v>1</v>
@@ -4667,7 +6158,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>353</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
@@ -4678,7 +6169,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>152</v>
+        <v>354</v>
       </c>
       <c r="C39" s="3">
         <v>1</v>
@@ -4689,7 +6180,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>153</v>
+        <v>355</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
@@ -4700,7 +6191,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>154</v>
+        <v>356</v>
       </c>
       <c r="C41" s="3">
         <v>1</v>
@@ -4711,7 +6202,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>155</v>
+        <v>357</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
@@ -4722,7 +6213,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>156</v>
+        <v>416</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
@@ -4733,7 +6224,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>157</v>
+        <v>358</v>
       </c>
       <c r="C44" s="3">
         <v>1</v>
@@ -4744,7 +6235,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>158</v>
+        <v>359</v>
       </c>
       <c r="C45" s="3">
         <v>1</v>
@@ -4755,7 +6246,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>159</v>
+        <v>360</v>
       </c>
       <c r="C46" s="3">
         <v>1</v>
@@ -4766,7 +6257,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>160</v>
+        <v>361</v>
       </c>
       <c r="C47" s="3">
         <v>1</v>
@@ -4777,7 +6268,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>161</v>
+        <v>362</v>
       </c>
       <c r="C48" s="3">
         <v>1</v>
@@ -4788,7 +6279,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>162</v>
+        <v>363</v>
       </c>
       <c r="C49" s="3">
         <v>1</v>
@@ -4799,7 +6290,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>163</v>
+        <v>364</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
@@ -4810,7 +6301,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>164</v>
+        <v>365</v>
       </c>
       <c r="C51" s="3">
         <v>1</v>
@@ -4821,7 +6312,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>165</v>
+        <v>366</v>
       </c>
       <c r="C52" s="3">
         <v>1</v>
@@ -4832,7 +6323,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>166</v>
+        <v>367</v>
       </c>
       <c r="C53" s="3">
         <v>1</v>
@@ -4843,7 +6334,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>167</v>
+        <v>368</v>
       </c>
       <c r="C54" s="3">
         <v>1</v>
@@ -4854,7 +6345,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>168</v>
+        <v>369</v>
       </c>
       <c r="C55" s="3">
         <v>1</v>
@@ -4865,7 +6356,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>370</v>
       </c>
       <c r="C56" s="3">
         <v>1</v>
@@ -4876,7 +6367,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>169</v>
+        <v>371</v>
       </c>
       <c r="C57" s="3">
         <v>1</v>
@@ -4887,7 +6378,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>170</v>
+        <v>415</v>
       </c>
       <c r="C58" s="3">
         <v>1</v>
@@ -4898,7 +6389,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>372</v>
       </c>
       <c r="C59" s="3">
         <v>1</v>
@@ -4909,7 +6400,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>171</v>
+        <v>373</v>
       </c>
       <c r="C60" s="3">
         <v>1</v>
@@ -4920,7 +6411,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>172</v>
+        <v>374</v>
       </c>
       <c r="C61" s="3">
         <v>1</v>
@@ -4931,7 +6422,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>173</v>
+        <v>375</v>
       </c>
       <c r="C62" s="3">
         <v>1</v>
@@ -4942,7 +6433,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>174</v>
+        <v>376</v>
       </c>
       <c r="C63" s="3">
         <v>1</v>
@@ -4953,7 +6444,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>175</v>
+        <v>377</v>
       </c>
       <c r="C64" s="3">
         <v>1</v>
@@ -4964,7 +6455,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>176</v>
+        <v>378</v>
       </c>
       <c r="C65" s="3">
         <v>1</v>
@@ -4975,7 +6466,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>177</v>
+        <v>379</v>
       </c>
       <c r="C66" s="3">
         <v>1</v>
@@ -4986,7 +6477,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>178</v>
+        <v>380</v>
       </c>
       <c r="C67" s="3">
         <v>1</v>
@@ -4997,7 +6488,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>179</v>
+        <v>381</v>
       </c>
       <c r="C68" s="3">
         <v>1</v>
@@ -5008,7 +6499,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>180</v>
+        <v>382</v>
       </c>
       <c r="C69" s="3">
         <v>1</v>
@@ -5019,7 +6510,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>181</v>
+        <v>383</v>
       </c>
       <c r="C70" s="3">
         <v>1</v>
@@ -5030,7 +6521,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>182</v>
+        <v>384</v>
       </c>
       <c r="C71" s="3">
         <v>1</v>
@@ -5041,7 +6532,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>183</v>
+        <v>385</v>
       </c>
       <c r="C72" s="3">
         <v>1</v>
@@ -5052,7 +6543,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>184</v>
+        <v>386</v>
       </c>
       <c r="C73" s="3">
         <v>1</v>
@@ -5063,7 +6554,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>185</v>
+        <v>387</v>
       </c>
       <c r="C74" s="3">
         <v>1</v>
@@ -5074,7 +6565,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>186</v>
+        <v>388</v>
       </c>
       <c r="C75" s="3">
         <v>1</v>
@@ -5085,7 +6576,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>187</v>
+        <v>389</v>
       </c>
       <c r="C76" s="3">
         <v>1</v>
@@ -5096,7 +6587,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>188</v>
+        <v>390</v>
       </c>
       <c r="C77" s="3">
         <v>1</v>
@@ -5107,7 +6598,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>189</v>
+        <v>391</v>
       </c>
       <c r="C78" s="3">
         <v>1</v>
@@ -5118,7 +6609,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>190</v>
+        <v>392</v>
       </c>
       <c r="C79" s="3">
         <v>1</v>
@@ -5129,7 +6620,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>191</v>
+        <v>393</v>
       </c>
       <c r="C80" s="3">
         <v>1</v>
@@ -5140,7 +6631,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>192</v>
+        <v>394</v>
       </c>
       <c r="C81" s="3">
         <v>1</v>
@@ -5151,7 +6642,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>193</v>
+        <v>395</v>
       </c>
       <c r="C82" s="3">
         <v>1</v>
@@ -5162,7 +6653,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>194</v>
+        <v>396</v>
       </c>
       <c r="C83" s="3">
         <v>1</v>
@@ -5173,7 +6664,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>195</v>
+        <v>397</v>
       </c>
       <c r="C84" s="3">
         <v>1</v>
@@ -5184,7 +6675,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>196</v>
+        <v>398</v>
       </c>
       <c r="C85" s="3">
         <v>1</v>
@@ -5195,7 +6686,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>197</v>
+        <v>399</v>
       </c>
       <c r="C86" s="3">
         <v>1</v>
@@ -5206,7 +6697,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>198</v>
+        <v>400</v>
       </c>
       <c r="C87" s="3">
         <v>1</v>
@@ -5217,7 +6708,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>199</v>
+        <v>401</v>
       </c>
       <c r="C88" s="3">
         <v>1</v>
@@ -5228,7 +6719,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>200</v>
+        <v>402</v>
       </c>
       <c r="C89" s="3">
         <v>1</v>
@@ -5239,7 +6730,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>6</v>
+        <v>403</v>
       </c>
       <c r="C90" s="3">
         <v>1</v>
@@ -5250,7 +6741,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>404</v>
       </c>
       <c r="C91" s="3">
         <v>1</v>
@@ -5261,7 +6752,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>201</v>
+        <v>405</v>
       </c>
       <c r="C92" s="3">
         <v>1</v>
@@ -5272,41 +6763,129 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>202</v>
+        <v>406</v>
       </c>
       <c r="C93" s="3">
         <v>1</v>
       </c>
     </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>407</v>
+      </c>
+      <c r="C94" s="3">
+        <v>1</v>
+      </c>
+    </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
+      <c r="A95" s="4">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>408</v>
+      </c>
+      <c r="C95" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>409</v>
+      </c>
+      <c r="C96" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>410</v>
+      </c>
+      <c r="C97" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>411</v>
+      </c>
+      <c r="C98" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>412</v>
+      </c>
+      <c r="C99" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>413</v>
+      </c>
+      <c r="C100" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="4">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>414</v>
+      </c>
+      <c r="C101" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C95">
-        <f>COUNTIFS(C1:C93,100%)</f>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
+      <c r="C103">
+        <f>COUNTIFS(C1:C101,100%)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C96">
+      <c r="C104">
         <f>COUNTIFS(C1:C92,"&gt;"&amp; 0%,C1:C92,"&lt;" &amp; 100%)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="4" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C97">
+      <c r="C105">
         <f>COUNTIFS(C1:C92,0%)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C93">
+  <conditionalFormatting sqref="C2:C101">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -5328,7 +6907,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5483,18 +7062,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.15217391304347827</v>
+        <v>0.16304347826086957</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>6.0869565217391308</v>
+        <v>6.5217391304347831</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -5546,23 +7125,23 @@
         <v>315</v>
       </c>
       <c r="C12" s="9">
-        <f>FluentValidation!A93</f>
-        <v>92</v>
+        <f>FluentValidation!C103</f>
+        <v>100</v>
       </c>
       <c r="D12" s="9">
-        <f>FluentValidation!C95</f>
-        <v>92</v>
+        <f>FluentValidation!C103</f>
+        <v>100</v>
       </c>
       <c r="E12" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F12" s="9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G12" s="12">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -5574,11 +7153,11 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9">
         <f>SUM(F4:F12)</f>
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>53.677781359551922</v>
+        <v>51.112563968247571</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -5587,7 +7166,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.24736304773987061</v>
+        <v>0.23884375686096995</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Se agregan cambios a la vista de préstamo
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -4785,8 +4785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5189,7 +5189,7 @@
         <v>451</v>
       </c>
       <c r="C36" s="3">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5702,7 +5702,7 @@
       </c>
       <c r="C85">
         <f>COUNTIFS(C2:C81,"&gt;"&amp; 0%,C2:C81,"&lt;" &amp; 100%)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="C86">
         <f>COUNTIFS(C2:C81,0%)</f>
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -6907,7 +6907,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7106,18 +7106,18 @@
         <v>83</v>
       </c>
       <c r="D11" s="9">
-        <v>4</v>
+        <v>4.55</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>4.8192771084337352E-2</v>
+        <v>5.4819277108433734E-2</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>5.7831325301204819</v>
+        <v>6.5783132530120483</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -7157,7 +7157,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>51.112563968247571</v>
+        <v>51.907744691139136</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7166,7 +7166,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.23884375686096995</v>
+        <v>0.24255955463149129</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Se agregan cambios para préstamo, proyecto, y tipo de préstamo
</commit_message>
<xml_diff>
--- a/Avances/Avances Controllers y DAOs.xlsx
+++ b/Avances/Avances Controllers y DAOs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -2080,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3139,7 +3139,7 @@
         <v>271</v>
       </c>
       <c r="D70" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" s="3"/>
     </row>
@@ -3154,7 +3154,7 @@
         <v>272</v>
       </c>
       <c r="D71" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="3"/>
     </row>
@@ -3498,7 +3498,7 @@
         <v>295</v>
       </c>
       <c r="D94" s="3">
-        <v>0</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
@@ -3508,7 +3508,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3518,7 +3518,7 @@
       <c r="C98" s="4"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -3528,7 +3528,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3570,8 +3570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3809,7 +3809,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="3">
-        <v>0</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -4381,7 +4381,7 @@
         <v>86</v>
       </c>
       <c r="C73" s="1">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -4425,7 +4425,7 @@
         <v>89</v>
       </c>
       <c r="C77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -4742,7 +4742,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4760,7 +4760,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4785,8 +4785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5156,7 +5156,7 @@
         <v>448</v>
       </c>
       <c r="C33" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5189,7 +5189,7 @@
         <v>451</v>
       </c>
       <c r="C36" s="3">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5702,7 +5702,7 @@
       </c>
       <c r="C85">
         <f>COUNTIFS(C2:C81,"&gt;"&amp; 0%,C2:C81,"&lt;" &amp; 100%)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="C86">
         <f>COUNTIFS(C2:C81,0%)</f>
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -6907,7 +6907,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7038,18 +7038,18 @@
       </c>
       <c r="D8" s="9">
         <f>Daos!C108</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.26923076923076922</v>
       </c>
       <c r="F8" s="9">
         <v>20</v>
       </c>
       <c r="G8" s="12">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>5.3846153846153841</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -7062,18 +7062,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.17391304347826086</v>
+        <v>0.19565217391304349</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>6.9565217391304346</v>
+        <v>7.8260869565217392</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7106,18 +7106,18 @@
         <v>83</v>
       </c>
       <c r="D11" s="9">
-        <v>4.8499999999999996</v>
+        <v>5</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>5.8433734939759029E-2</v>
+        <v>6.0240963855421686E-2</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>7.0120481927710836</v>
+        <v>7.2289156626506026</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -7157,7 +7157,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>52.96856993190152</v>
+        <v>54.439618003787722</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7166,7 +7166,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.24751668192477347</v>
+        <v>0.25439073833545667</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>